<commit_message>
Much Added features, including order log, config files, and menu generator
</commit_message>
<xml_diff>
--- a/Beijing Inn Order System/AddressList.xlsx
+++ b/Beijing Inn Order System/AddressList.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$3000</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$4025</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12072" uniqueCount="5704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12072" uniqueCount="5705">
   <si>
     <t>Rochester</t>
   </si>
@@ -17135,6 +17135,9 @@
   </si>
   <si>
     <t>ME5 0BA</t>
+  </si>
+  <si>
+    <t>Brompton High Street</t>
   </si>
 </sst>
 </file>
@@ -17955,10 +17958,14 @@
   <dimension ref="A2:E4025"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3093" sqref="J3093"/>
+      <selection activeCell="B4026" sqref="B4026"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -44264,10 +44271,10 @@
         <v>2120</v>
       </c>
       <c r="B1549" t="s">
-        <v>5</v>
+        <v>5704</v>
       </c>
       <c r="C1549" t="s">
-        <v>2113</v>
+        <v>288</v>
       </c>
       <c r="D1549">
         <v>51.391669880000002</v>
@@ -86369,7 +86376,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E3000"/>
+  <autoFilter ref="A2:E4025"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>